<commit_message>
Change Market Gap colors
</commit_message>
<xml_diff>
--- a/Presentations/DesignPres/marketGap.xlsx
+++ b/Presentations/DesignPres/marketGap.xlsx
@@ -326,7 +326,7 @@
             <a:noFill/>
             <a:ln w="38100">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -713,11 +713,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-419086912"/>
-        <c:axId val="-419076576"/>
+        <c:axId val="1813269744"/>
+        <c:axId val="1813265392"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-419086912"/>
+        <c:axId val="1813269744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -825,12 +825,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-419076576"/>
+        <c:crossAx val="1813265392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-419076576"/>
+        <c:axId val="1813265392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500"/>
@@ -930,7 +930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-419086912"/>
+        <c:crossAx val="1813269744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1574,7 +1574,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8654143" cy="6272893"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>

<commit_message>
Change market gap color
</commit_message>
<xml_diff>
--- a/Presentations/DesignPres/marketGap.xlsx
+++ b/Presentations/DesignPres/marketGap.xlsx
@@ -655,11 +655,11 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="0070C0"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -713,11 +713,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="1813269744"/>
-        <c:axId val="1813265392"/>
+        <c:axId val="1907773264"/>
+        <c:axId val="1907774896"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="1813269744"/>
+        <c:axId val="1907773264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -825,12 +825,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1813265392"/>
+        <c:crossAx val="1907774896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1813265392"/>
+        <c:axId val="1907774896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500"/>
@@ -930,7 +930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1813269744"/>
+        <c:crossAx val="1907773264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
Update Market Gap Formatting
</commit_message>
<xml_diff>
--- a/Presentations/DesignPres/marketGap.xlsx
+++ b/Presentations/DesignPres/marketGap.xlsx
@@ -326,7 +326,7 @@
             <a:noFill/>
             <a:ln w="38100">
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -559,7 +559,7 @@
             <a:noFill/>
             <a:ln w="38100">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -655,11 +655,11 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -713,17 +713,30 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="1907773264"/>
-        <c:axId val="1907774896"/>
+        <c:axId val="-1203466560"/>
+        <c:axId val="-1203469280"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="1907773264"/>
+        <c:axId val="-1203466560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -796,10 +809,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -825,12 +835,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1907774896"/>
+        <c:crossAx val="-1203469280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1907774896"/>
+        <c:axId val="-1203469280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500"/>
@@ -838,6 +848,19 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -906,7 +929,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -930,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1907773264"/>
+        <c:crossAx val="-1203466560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>